<commit_message>
last of homework 1 + a few minor tweaks
</commit_message>
<xml_diff>
--- a/homework_graded/homework_all_grades.xlsx
+++ b/homework_graded/homework_all_grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/homework_graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBAC50D-E19F-934D-860D-D761FA6D553F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EE5AE0-FD2E-AE4A-9F6B-F5FAA3F1068A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="1560" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
+    <workbookView xWindow="4920" yWindow="760" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Al Qassab, Omar</t>
   </si>
@@ -474,7 +474,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,13 +537,17 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -597,7 +601,9 @@
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tidy up here and there
</commit_message>
<xml_diff>
--- a/homework_graded/homework_all_grades.xlsx
+++ b/homework_graded/homework_all_grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/homework_graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EE5AE0-FD2E-AE4A-9F6B-F5FAA3F1068A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E461BC1-633C-DE4F-ABB3-8019EF273FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="760" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
+    <workbookView xWindow="4360" yWindow="3960" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Al Qassab, Omar</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>good</t>
+  </si>
+  <si>
+    <t>due_2021-09-07</t>
   </si>
 </sst>
 </file>
@@ -474,17 +477,18 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="4">
-        <v>44446</v>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
upload the last of homework 2
</commit_message>
<xml_diff>
--- a/homework_graded/homework_all_grades.xlsx
+++ b/homework_graded/homework_all_grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/homework_graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B62CC50-8D36-C14F-854B-B2C7116E1912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD6444E-8A9F-2041-80E6-DF7B84021937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="1400" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,6 +518,9 @@
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C3" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">

</xml_diff>

<commit_message>
update key for w4 r1, update key for hw3, add graded hw3
</commit_message>
<xml_diff>
--- a/homework_graded/homework_all_grades.xlsx
+++ b/homework_graded/homework_all_grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/homework_graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD6444E-8A9F-2041-80E6-DF7B84021937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E694C49-D56A-5B44-80DE-08A30C2FFD49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="1400" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
+    <workbookView xWindow="2720" yWindow="1540" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Al Qassab, Omar</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>did not turn in</t>
+  </si>
+  <si>
+    <t>due_2021-09-23</t>
   </si>
 </sst>
 </file>
@@ -480,27 +483,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1D7807-2F99-5E49-B90D-00EBE2C67A04}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -510,8 +516,11 @@
       <c r="C2" s="1">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -521,8 +530,11 @@
       <c r="C3" s="1">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -532,8 +544,11 @@
       <c r="C4" s="1">
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -543,8 +558,11 @@
       <c r="C5" s="1">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -554,8 +572,11 @@
       <c r="C6" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -565,8 +586,11 @@
       <c r="C7" s="1">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -576,8 +600,11 @@
       <c r="C8" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -587,8 +614,11 @@
       <c r="C9" s="1">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -598,8 +628,11 @@
       <c r="C10" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -609,8 +642,11 @@
       <c r="C11" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -620,8 +656,11 @@
       <c r="C12" s="1">
         <v>99</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -631,8 +670,11 @@
       <c r="C13" s="1">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -642,8 +684,11 @@
       <c r="C14" s="1">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D14" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -653,8 +698,11 @@
       <c r="C15" s="1">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -663,6 +711,9 @@
       </c>
       <c r="C16" s="1">
         <v>99</v>
+      </c>
+      <c r="D16" s="1">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hw 8 partial + index 9
</commit_message>
<xml_diff>
--- a/homework_graded/homework_all_grades.xlsx
+++ b/homework_graded/homework_all_grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/homework_graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817AB5EF-732C-2944-9A96-6421D46002A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60426B3A-15AD-B34A-8833-6689D5E530B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="1540" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Al Qassab, Omar</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>hw7</t>
+  </si>
+  <si>
+    <t>hw8</t>
   </si>
 </sst>
 </file>
@@ -502,20 +505,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1D7807-2F99-5E49-B90D-00EBE2C67A04}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
@@ -537,8 +540,11 @@
       <c r="H1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -564,7 +570,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -589,8 +595,11 @@
       <c r="H3" s="1">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -615,8 +624,11 @@
       <c r="H4" s="1">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -641,8 +653,11 @@
       <c r="H5" s="1">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -665,7 +680,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -690,8 +705,11 @@
       <c r="H7" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -716,8 +734,11 @@
       <c r="H8" s="1">
         <v>92</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -742,8 +763,11 @@
       <c r="H9" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -768,8 +792,11 @@
       <c r="H10" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -794,8 +821,11 @@
       <c r="H11" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -820,8 +850,11 @@
       <c r="H12" s="1">
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -847,7 +880,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -873,7 +906,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -899,7 +932,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
update graded hw files
</commit_message>
<xml_diff>
--- a/homework_graded/homework_all_grades.xlsx
+++ b/homework_graded/homework_all_grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/homework_graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60426B3A-15AD-B34A-8833-6689D5E530B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491A7320-F174-0247-82DD-CBFFABA0427D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="1540" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Al Qassab, Omar</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>hw8</t>
+  </si>
+  <si>
+    <t>hw9</t>
+  </si>
+  <si>
+    <t>hw10</t>
   </si>
 </sst>
 </file>
@@ -505,20 +511,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1D7807-2F99-5E49-B90D-00EBE2C67A04}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
@@ -543,8 +550,14 @@
       <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -566,11 +579,17 @@
       <c r="G2" s="1">
         <v>99</v>
       </c>
-      <c r="H2" s="1">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="6">
+        <v>99</v>
+      </c>
+      <c r="I2" s="6">
+        <v>99</v>
+      </c>
+      <c r="J2" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -592,14 +611,17 @@
       <c r="G3" s="1">
         <v>99</v>
       </c>
-      <c r="H3" s="1">
-        <v>99</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="H3" s="6">
+        <v>99</v>
+      </c>
+      <c r="I3" s="6">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -621,14 +643,17 @@
       <c r="G4" s="1">
         <v>100</v>
       </c>
-      <c r="H4" s="1">
-        <v>98</v>
-      </c>
-      <c r="I4" s="1">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="6">
+        <v>98</v>
+      </c>
+      <c r="I4" s="6">
+        <v>99</v>
+      </c>
+      <c r="J4" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -650,14 +675,17 @@
       <c r="G5" s="1">
         <v>94</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="6">
         <v>93</v>
       </c>
-      <c r="I5" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="6">
+        <v>98</v>
+      </c>
+      <c r="J5" s="6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -679,8 +707,17 @@
       <c r="G6" s="1">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="6">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -702,14 +739,17 @@
       <c r="G7" s="1">
         <v>100</v>
       </c>
-      <c r="H7" s="1">
-        <v>100</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H7" s="6">
+        <v>100</v>
+      </c>
+      <c r="I7" s="6">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -731,14 +771,17 @@
       <c r="G8" s="1">
         <v>100</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="6">
         <v>92</v>
       </c>
-      <c r="I8" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="6">
+        <v>100</v>
+      </c>
+      <c r="J8" s="6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -760,14 +803,17 @@
       <c r="G9" s="1">
         <v>100</v>
       </c>
-      <c r="H9" s="1">
-        <v>100</v>
-      </c>
-      <c r="I9" s="1">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="6">
+        <v>100</v>
+      </c>
+      <c r="I9" s="6">
+        <v>99</v>
+      </c>
+      <c r="J9" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -789,14 +835,17 @@
       <c r="G10" s="1">
         <v>100</v>
       </c>
-      <c r="H10" s="1">
-        <v>100</v>
-      </c>
-      <c r="I10" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="6">
+        <v>100</v>
+      </c>
+      <c r="I10" s="6">
+        <v>100</v>
+      </c>
+      <c r="J10" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -818,14 +867,17 @@
       <c r="G11" s="1">
         <v>100</v>
       </c>
-      <c r="H11" s="1">
-        <v>100</v>
-      </c>
-      <c r="I11" s="1">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="6">
+        <v>100</v>
+      </c>
+      <c r="I11" s="6">
+        <v>99</v>
+      </c>
+      <c r="J11" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -847,14 +899,17 @@
       <c r="G12" s="1">
         <v>100</v>
       </c>
-      <c r="H12" s="1">
-        <v>98</v>
-      </c>
-      <c r="I12" s="1">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="6">
+        <v>98</v>
+      </c>
+      <c r="I12" s="6">
+        <v>99</v>
+      </c>
+      <c r="J12" s="6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -876,11 +931,17 @@
       <c r="G13" s="1">
         <v>96</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="6">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="6">
+        <v>89</v>
+      </c>
+      <c r="J13" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -902,11 +963,17 @@
       <c r="G14" s="1">
         <v>100</v>
       </c>
-      <c r="H14" s="1">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="6">
+        <v>99</v>
+      </c>
+      <c r="I14" s="6">
+        <v>99</v>
+      </c>
+      <c r="J14" s="6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -928,11 +995,17 @@
       <c r="G15" s="1">
         <v>99</v>
       </c>
-      <c r="H15" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="6">
+        <v>98</v>
+      </c>
+      <c r="I15" s="6">
+        <v>95</v>
+      </c>
+      <c r="J15" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -954,7 +1027,13 @@
       <c r="G16" s="1">
         <v>100</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="6">
+        <v>100</v>
+      </c>
+      <c r="I16" s="6">
+        <v>99</v>
+      </c>
+      <c r="J16" s="6">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final final + hw11
</commit_message>
<xml_diff>
--- a/homework_graded/homework_all_grades.xlsx
+++ b/homework_graded/homework_all_grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/homework_graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35DCB6E-EE18-0D45-AE3B-A8F90F749A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8F8966-83EA-B444-B22C-ABFDFC86786D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="1540" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,6 +603,9 @@
       <c r="K2" s="1">
         <v>100</v>
       </c>
+      <c r="L2" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -638,6 +641,9 @@
       <c r="K3" s="1">
         <v>97</v>
       </c>
+      <c r="L3" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -673,6 +679,9 @@
       <c r="K4" s="1">
         <v>99</v>
       </c>
+      <c r="L4" s="1">
+        <v>99</v>
+      </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -708,6 +717,9 @@
       <c r="K5" s="1">
         <v>93</v>
       </c>
+      <c r="L5" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -743,6 +755,9 @@
       <c r="K6" s="1">
         <v>98</v>
       </c>
+      <c r="L6" s="1">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -778,6 +793,9 @@
       <c r="K7" s="1">
         <v>99</v>
       </c>
+      <c r="L7" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -813,6 +831,9 @@
       <c r="K8" s="1">
         <v>100</v>
       </c>
+      <c r="L8" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -848,6 +869,9 @@
       <c r="K9" s="1">
         <v>99</v>
       </c>
+      <c r="L9" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -881,6 +905,9 @@
         <v>100</v>
       </c>
       <c r="K10" s="1">
+        <v>100</v>
+      </c>
+      <c r="L10" s="1">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upload last hw grades
</commit_message>
<xml_diff>
--- a/homework_graded/homework_all_grades.xlsx
+++ b/homework_graded/homework_all_grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/homework_graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C05E86-036E-1A4C-9101-551B7F8B1A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B0E505-F8C9-504C-9C68-2690F23413B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="1540" windowWidth="27640" windowHeight="16940" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
@@ -589,7 +589,7 @@
   <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,9 +786,12 @@
       <c r="M3" s="1">
         <v>98</v>
       </c>
+      <c r="N3" s="1">
+        <v>100</v>
+      </c>
       <c r="O3" s="9">
         <f t="shared" ref="O3:O16" si="0">LARGE(C3:N3,1)</f>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P3" s="9">
         <f t="shared" ref="P3:P16" si="1">LARGE(C3:N3,2)</f>
@@ -796,7 +799,7 @@
       </c>
       <c r="Q3" s="9">
         <f t="shared" ref="Q3:Q16" si="2">LARGE(C3:N3,3)</f>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R3" s="9">
         <f t="shared" ref="R3:R16" si="3">LARGE(C3:N3,4)</f>
@@ -816,7 +819,7 @@
       </c>
       <c r="V3" s="9">
         <f t="shared" ref="V3:V16" si="7">LARGE(C3:N3,8)</f>
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W3" s="9">
         <f t="shared" ref="W3:W16" si="8">LARGE(C3:N3,9)</f>
@@ -824,7 +827,7 @@
       </c>
       <c r="X3" s="9">
         <f t="shared" ref="X3:X16" si="9">LARGE(C3:N3,10)</f>
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="Y3" s="8">
         <f t="shared" ref="Y3:Y16" si="10">IF(ROUND(AVERAGE(O3:X3),0)&gt;100,100,ROUND(AVERAGE(O3:X3),0))</f>
@@ -871,6 +874,9 @@
       <c r="M4" s="1">
         <v>98</v>
       </c>
+      <c r="N4" s="1">
+        <v>95</v>
+      </c>
       <c r="O4" s="9">
         <f t="shared" si="0"/>
         <v>104</v>
@@ -956,6 +962,9 @@
       <c r="M5" s="1">
         <v>97</v>
       </c>
+      <c r="N5" s="1">
+        <v>89</v>
+      </c>
       <c r="O5" s="9">
         <f t="shared" si="0"/>
         <v>109</v>
@@ -1129,6 +1138,9 @@
       <c r="M7" s="1">
         <v>100</v>
       </c>
+      <c r="N7" s="1">
+        <v>100</v>
+      </c>
       <c r="O7" s="9">
         <f t="shared" si="0"/>
         <v>109</v>
@@ -1155,7 +1167,7 @@
       </c>
       <c r="U7" s="9">
         <f t="shared" si="6"/>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="V7" s="9">
         <f t="shared" si="7"/>
@@ -1163,11 +1175,11 @@
       </c>
       <c r="W7" s="9">
         <f t="shared" si="8"/>
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X7" s="9">
         <f t="shared" si="9"/>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Y7" s="8">
         <f t="shared" si="10"/>
@@ -1214,6 +1226,9 @@
       <c r="M8" s="1">
         <v>100</v>
       </c>
+      <c r="N8" s="1">
+        <v>100</v>
+      </c>
       <c r="O8" s="9">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -1240,23 +1255,23 @@
       </c>
       <c r="U8" s="9">
         <f t="shared" si="6"/>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="V8" s="9">
         <f t="shared" si="7"/>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="W8" s="9">
         <f t="shared" si="8"/>
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="X8" s="9">
         <f t="shared" si="9"/>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y8" s="8">
         <f t="shared" si="10"/>
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1299,6 +1314,9 @@
       <c r="M9" s="1">
         <v>99</v>
       </c>
+      <c r="N9" s="1">
+        <v>100</v>
+      </c>
       <c r="O9" s="9">
         <f t="shared" si="0"/>
         <v>109</v>
@@ -1321,7 +1339,7 @@
       </c>
       <c r="T9" s="9">
         <f t="shared" si="5"/>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="U9" s="9">
         <f t="shared" si="6"/>
@@ -1337,7 +1355,7 @@
       </c>
       <c r="X9" s="9">
         <f t="shared" si="9"/>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Y9" s="8">
         <f t="shared" si="10"/>
@@ -1384,6 +1402,9 @@
       <c r="M10" s="1">
         <v>100</v>
       </c>
+      <c r="N10" s="1">
+        <v>100</v>
+      </c>
       <c r="O10" s="9">
         <f t="shared" si="0"/>
         <v>110</v>
@@ -1469,6 +1490,9 @@
       <c r="M11" s="1">
         <v>100</v>
       </c>
+      <c r="N11" s="1">
+        <v>100</v>
+      </c>
       <c r="O11" s="9">
         <f t="shared" si="0"/>
         <v>110</v>
@@ -1507,7 +1531,7 @@
       </c>
       <c r="X11" s="9">
         <f t="shared" si="9"/>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Y11" s="8">
         <f t="shared" si="10"/>
@@ -1554,6 +1578,9 @@
       <c r="M12" s="1">
         <v>100</v>
       </c>
+      <c r="N12" s="1">
+        <v>100</v>
+      </c>
       <c r="O12" s="9">
         <f t="shared" si="0"/>
         <v>108</v>
@@ -1576,7 +1603,7 @@
       </c>
       <c r="T12" s="9">
         <f t="shared" si="5"/>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="U12" s="9">
         <f t="shared" si="6"/>
@@ -1584,7 +1611,7 @@
       </c>
       <c r="V12" s="9">
         <f t="shared" si="7"/>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="W12" s="9">
         <f t="shared" si="8"/>
@@ -1639,6 +1666,9 @@
       <c r="M13" s="1">
         <v>83</v>
       </c>
+      <c r="N13" s="1">
+        <v>90</v>
+      </c>
       <c r="O13" s="9">
         <f t="shared" si="0"/>
         <v>101</v>
@@ -1677,7 +1707,7 @@
       </c>
       <c r="X13" s="9">
         <f t="shared" si="9"/>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y13" s="8">
         <f t="shared" si="10"/>
@@ -1724,6 +1754,9 @@
       <c r="M14" s="1">
         <v>98</v>
       </c>
+      <c r="N14" s="1">
+        <v>95</v>
+      </c>
       <c r="O14" s="9">
         <f t="shared" si="0"/>
         <v>108</v>
@@ -1806,6 +1839,12 @@
       <c r="L15" s="1">
         <v>93</v>
       </c>
+      <c r="M15" s="1">
+        <v>78</v>
+      </c>
+      <c r="N15" s="1">
+        <v>90</v>
+      </c>
       <c r="O15" s="9">
         <f t="shared" si="0"/>
         <v>108</v>
@@ -1844,11 +1883,11 @@
       </c>
       <c r="X15" s="9">
         <f t="shared" si="9"/>
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="Y15" s="8">
         <f t="shared" si="10"/>
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1891,6 +1930,9 @@
       <c r="M16" s="1">
         <v>100</v>
       </c>
+      <c r="N16" s="1">
+        <v>100</v>
+      </c>
       <c r="O16" s="9">
         <f t="shared" si="0"/>
         <v>109</v>
@@ -1921,7 +1963,7 @@
       </c>
       <c r="V16" s="9">
         <f t="shared" si="7"/>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="W16" s="9">
         <f t="shared" si="8"/>

</xml_diff>

<commit_message>
update final homework and grades
</commit_message>
<xml_diff>
--- a/homework_graded/homework_all_grades.xlsx
+++ b/homework_graded/homework_all_grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/homework_graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D133DA-DD7C-634B-B781-30E808605AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16451701-2B39-0A4E-A11D-7DF72632D735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
@@ -256,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -316,17 +316,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -348,8 +337,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -365,6 +352,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1350,8 +1339,8 @@
   <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z12" sqref="Z12"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1410,18 +1399,18 @@
       <c r="N1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="26"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="24"/>
       <c r="Y1" s="13" t="s">
         <v>42</v>
       </c>
@@ -1440,7 +1429,7 @@
       <c r="AD1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AE1" s="17" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1527,11 +1516,13 @@
         <f>LARGE(C2:N2,10)</f>
         <v>97</v>
       </c>
-      <c r="Y2" s="23">
+      <c r="Y2" s="21">
         <f>IF(ROUND(AVERAGE(O2:X2),0)&gt;100,100,ROUND(AVERAGE(O2:X2),0))</f>
         <v>100</v>
       </c>
-      <c r="Z2" s="21"/>
+      <c r="Z2" s="19">
+        <v>100</v>
+      </c>
       <c r="AA2" s="14">
         <v>88</v>
       </c>
@@ -1540,10 +1531,10 @@
       </c>
       <c r="AC2" s="10">
         <f xml:space="preserve"> Y2*0.7 + Z2*0.1 + AA2*0.1 + AB2*0.1</f>
-        <v>88.8</v>
+        <v>98.8</v>
       </c>
       <c r="AD2" s="12"/>
-      <c r="AE2" s="18" t="s">
+      <c r="AE2" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1630,11 +1621,11 @@
         <f t="shared" ref="X3:X16" si="9">LARGE(C3:N3,10)</f>
         <v>97</v>
       </c>
-      <c r="Y3" s="23">
+      <c r="Y3" s="21">
         <f t="shared" ref="Y3:Y16" si="10">IF(ROUND(AVERAGE(O3:X3),0)&gt;100,100,ROUND(AVERAGE(O3:X3),0))</f>
         <v>98</v>
       </c>
-      <c r="Z3" s="21">
+      <c r="Z3" s="19">
         <v>99</v>
       </c>
       <c r="AA3" s="14">
@@ -1648,7 +1639,7 @@
         <v>95.1</v>
       </c>
       <c r="AD3" s="12"/>
-      <c r="AE3" s="18" t="s">
+      <c r="AE3" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1735,11 +1726,13 @@
         <f t="shared" si="9"/>
         <v>95</v>
       </c>
-      <c r="Y4" s="23">
+      <c r="Y4" s="21">
         <f t="shared" si="10"/>
         <v>99</v>
       </c>
-      <c r="Z4" s="21"/>
+      <c r="Z4" s="19">
+        <v>100</v>
+      </c>
       <c r="AA4" s="14">
         <v>86</v>
       </c>
@@ -1748,10 +1741,10 @@
       </c>
       <c r="AC4" s="10">
         <f t="shared" si="11"/>
-        <v>87.899999999999991</v>
+        <v>97.899999999999991</v>
       </c>
       <c r="AD4" s="12"/>
-      <c r="AE4" s="18" t="s">
+      <c r="AE4" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1838,11 +1831,13 @@
         <f t="shared" si="9"/>
         <v>93</v>
       </c>
-      <c r="Y5" s="23">
+      <c r="Y5" s="21">
         <f t="shared" si="10"/>
         <v>97</v>
       </c>
-      <c r="Z5" s="21"/>
+      <c r="Z5" s="19">
+        <v>87</v>
+      </c>
       <c r="AA5" s="14">
         <v>71</v>
       </c>
@@ -1851,10 +1846,10 @@
       </c>
       <c r="AC5" s="10">
         <f t="shared" si="11"/>
-        <v>84.999999999999986</v>
+        <v>93.699999999999989</v>
       </c>
       <c r="AD5" s="12"/>
-      <c r="AE5" s="18" t="s">
+      <c r="AE5" s="16" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1941,11 +1936,11 @@
         <f t="shared" si="9"/>
         <v>79</v>
       </c>
-      <c r="Y6" s="23">
+      <c r="Y6" s="21">
         <f t="shared" si="10"/>
         <v>93</v>
       </c>
-      <c r="Z6" s="21"/>
+      <c r="Z6" s="19"/>
       <c r="AA6" s="14">
         <v>63</v>
       </c>
@@ -1957,7 +1952,7 @@
         <v>81.399999999999991</v>
       </c>
       <c r="AD6" s="12"/>
-      <c r="AE6" s="18" t="s">
+      <c r="AE6" s="16" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2044,11 +2039,13 @@
         <f t="shared" si="9"/>
         <v>97</v>
       </c>
-      <c r="Y7" s="23">
+      <c r="Y7" s="21">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="Z7" s="21"/>
+      <c r="Z7" s="19">
+        <v>100</v>
+      </c>
       <c r="AA7" s="14">
         <v>73</v>
       </c>
@@ -2057,10 +2054,10 @@
       </c>
       <c r="AC7" s="10">
         <f t="shared" si="11"/>
-        <v>87.3</v>
+        <v>97.3</v>
       </c>
       <c r="AD7" s="12"/>
-      <c r="AE7" s="18" t="s">
+      <c r="AE7" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2147,11 +2144,13 @@
         <f t="shared" si="9"/>
         <v>93</v>
       </c>
-      <c r="Y8" s="23">
+      <c r="Y8" s="21">
         <f t="shared" si="10"/>
         <v>99</v>
       </c>
-      <c r="Z8" s="21"/>
+      <c r="Z8" s="19">
+        <v>93</v>
+      </c>
       <c r="AA8" s="14">
         <v>93</v>
       </c>
@@ -2160,10 +2159,10 @@
       </c>
       <c r="AC8" s="10">
         <f t="shared" si="11"/>
-        <v>88.6</v>
+        <v>97.899999999999991</v>
       </c>
       <c r="AD8" s="12"/>
-      <c r="AE8" s="18" t="s">
+      <c r="AE8" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2250,12 +2249,12 @@
         <f t="shared" si="9"/>
         <v>99</v>
       </c>
-      <c r="Y9" s="23">
+      <c r="Y9" s="21">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="Z9" s="21">
-        <v>99</v>
+      <c r="Z9" s="19">
+        <v>98</v>
       </c>
       <c r="AA9" s="14">
         <v>91</v>
@@ -2265,10 +2264,10 @@
       </c>
       <c r="AC9" s="10">
         <f t="shared" si="11"/>
-        <v>99</v>
+        <v>98.899999999999991</v>
       </c>
       <c r="AD9" s="12"/>
-      <c r="AE9" s="18" t="s">
+      <c r="AE9" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2355,11 +2354,11 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="Y10" s="23">
+      <c r="Y10" s="21">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="Z10" s="22"/>
+      <c r="Z10" s="20"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5">
         <v>100</v>
@@ -2369,7 +2368,7 @@
         <v>80</v>
       </c>
       <c r="AD10" s="5"/>
-      <c r="AE10" s="20" t="s">
+      <c r="AE10" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2456,11 +2455,11 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="Y11" s="23">
+      <c r="Y11" s="21">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="Z11" s="21"/>
+      <c r="Z11" s="19"/>
       <c r="AA11" s="14">
         <v>74</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>87.4</v>
       </c>
       <c r="AD11" s="12"/>
-      <c r="AE11" s="18" t="s">
+      <c r="AE11" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2559,12 +2558,12 @@
         <f t="shared" si="9"/>
         <v>98</v>
       </c>
-      <c r="Y12" s="23">
+      <c r="Y12" s="21">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="Z12" s="21">
-        <v>99</v>
+      <c r="Z12" s="19">
+        <v>98</v>
       </c>
       <c r="AA12" s="14">
         <v>73</v>
@@ -2574,10 +2573,10 @@
       </c>
       <c r="AC12" s="10">
         <f t="shared" si="11"/>
-        <v>97.2</v>
+        <v>97.1</v>
       </c>
       <c r="AD12" s="12"/>
-      <c r="AE12" s="18" t="s">
+      <c r="AE12" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2664,11 +2663,11 @@
         <f t="shared" si="9"/>
         <v>90</v>
       </c>
-      <c r="Y13" s="23">
+      <c r="Y13" s="21">
         <f t="shared" si="10"/>
         <v>96</v>
       </c>
-      <c r="Z13" s="22"/>
+      <c r="Z13" s="20"/>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5">
         <v>100</v>
@@ -2678,7 +2677,7 @@
         <v>77.199999999999989</v>
       </c>
       <c r="AD13" s="5"/>
-      <c r="AE13" s="20" t="s">
+      <c r="AE13" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2765,11 +2764,11 @@
         <f t="shared" si="9"/>
         <v>98</v>
       </c>
-      <c r="Y14" s="23">
+      <c r="Y14" s="21">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="Z14" s="21">
+      <c r="Z14" s="19">
         <v>99</v>
       </c>
       <c r="AA14" s="14">
@@ -2783,7 +2782,7 @@
         <v>98.4</v>
       </c>
       <c r="AD14" s="12"/>
-      <c r="AE14" s="18" t="s">
+      <c r="AE14" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2870,11 +2869,11 @@
         <f t="shared" si="9"/>
         <v>90</v>
       </c>
-      <c r="Y15" s="23">
+      <c r="Y15" s="21">
         <f t="shared" si="10"/>
         <v>98</v>
       </c>
-      <c r="Z15" s="21">
+      <c r="Z15" s="19">
         <v>98</v>
       </c>
       <c r="AA15" s="14">
@@ -2888,7 +2887,7 @@
         <v>96.3</v>
       </c>
       <c r="AD15" s="12"/>
-      <c r="AE15" s="18" t="s">
+      <c r="AE15" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2975,11 +2974,13 @@
         <f t="shared" si="9"/>
         <v>99</v>
       </c>
-      <c r="Y16" s="23">
+      <c r="Y16" s="21">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="Z16" s="21"/>
+      <c r="Z16" s="19">
+        <v>100</v>
+      </c>
       <c r="AA16" s="14">
         <v>70</v>
       </c>
@@ -2988,10 +2989,10 @@
       </c>
       <c r="AC16" s="10">
         <f t="shared" si="11"/>
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="AD16" s="12"/>
-      <c r="AE16" s="18" t="s">
+      <c r="AE16" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2999,19 +3000,19 @@
       <c r="A17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="Y17" s="15">
+      <c r="Y17" s="25">
         <v>0.7</v>
       </c>
-      <c r="Z17" s="15">
+      <c r="Z17" s="25">
         <v>0.1</v>
       </c>
-      <c r="AA17" s="16">
+      <c r="AA17" s="26">
         <v>0.1</v>
       </c>
-      <c r="AB17" s="17">
+      <c r="AB17" s="26">
         <v>0.1</v>
       </c>
-      <c r="AC17" s="16">
+      <c r="AC17" s="26">
         <f>SUM(Y17:AB17)</f>
         <v>0.99999999999999989</v>
       </c>

</xml_diff>